<commit_message>
Quotations linked to customers
</commit_message>
<xml_diff>
--- a/Project documents/elaboration-phase/20161016_genormaliseerde_database_structuur.xlsx
+++ b/Project documents/elaboration-phase/20161016_genormaliseerde_database_structuur.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="80">
   <si>
     <t>Customer_ID</t>
   </si>
@@ -195,9 +195,6 @@
   </si>
   <si>
     <t>tbl_quotations</t>
-  </si>
-  <si>
-    <t>•Quotation_ID</t>
   </si>
   <si>
     <t>Ledger account number</t>
@@ -650,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,12 +728,12 @@
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
@@ -751,7 +748,7 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
@@ -776,22 +773,22 @@
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
@@ -816,12 +813,12 @@
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
@@ -856,7 +853,7 @@
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
@@ -866,12 +863,12 @@
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
@@ -891,7 +888,7 @@
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
@@ -932,6 +929,9 @@
       <c r="D53" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="F53" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B55" s="4" t="s">
@@ -940,6 +940,9 @@
       <c r="D55" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="F55" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
@@ -948,6 +951,9 @@
       <c r="D56" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="F56" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
@@ -956,6 +962,9 @@
       <c r="D57" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="F57" s="6" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
@@ -964,13 +973,19 @@
       <c r="D58" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="F58" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
@@ -978,7 +993,10 @@
         <v>5</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
@@ -1007,7 +1025,7 @@
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B64" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>37</v>
@@ -1015,7 +1033,7 @@
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B65" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>38</v>
@@ -1034,23 +1052,23 @@
         <v>12</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B68" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D69" s="7" t="s">
-        <v>80</v>
+      <c r="D69" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
@@ -1058,7 +1076,7 @@
         <v>10</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
@@ -1066,47 +1084,32 @@
         <v>14</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B73" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B74" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B75" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B76" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1171,7 +1174,7 @@
         <v>0</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F83" s="4" t="s">
         <v>49</v>
@@ -1194,7 +1197,7 @@
         <v>44</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="J84" s="4" t="s">
         <v>19</v>
@@ -1208,13 +1211,13 @@
         <v>29</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.25">
@@ -1225,10 +1228,10 @@
         <v>30</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J86" s="1" t="s">
         <v>13</v>
@@ -1253,10 +1256,10 @@
         <v>5</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>11</v>
@@ -1267,7 +1270,7 @@
         <v>6</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>27</v>
@@ -1278,7 +1281,7 @@
         <v>7</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.25">
@@ -1289,12 +1292,12 @@
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B92" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B93" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.25">
@@ -1309,7 +1312,7 @@
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B96" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
@@ -1334,22 +1337,22 @@
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>